<commit_message>
atualizando documentação e backlog
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog.xlsx
+++ b/Documentação/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/fabricio_ferreira_sptech_school/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{607989F4-54B1-40AD-9008-3F3AC558A12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59B191D3-C18D-4217-81EC-CB1DA6A33E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6A767852-0E7C-48FF-B159-3DC06DD3FC16}"/>
+    <workbookView minimized="1" xWindow="3630" yWindow="3015" windowWidth="21600" windowHeight="11295" xr2:uid="{6A767852-0E7C-48FF-B159-3DC06DD3FC16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>PROJECT BACKLOG</t>
   </si>
@@ -257,10 +257,22 @@
     <t xml:space="preserve">Demonstração de um servidor local funcional juntamente com testagem das aplicações em outros sistemas operacionais </t>
   </si>
   <si>
-    <t>Fase de testagem</t>
-  </si>
-  <si>
-    <t>Aplicação do sistema em outras máquinas somada a correção de possíveis erros</t>
+    <t>Função para indicar/controlar status da incubadora</t>
+  </si>
+  <si>
+    <t>Botão na tela Gerenciar para indicar a saída do recém nascido de3 uma incubadora.</t>
+  </si>
+  <si>
+    <t>Assistente virtul</t>
+  </si>
+  <si>
+    <t>Assistente virtual baseado na Inteligência Artificial Gemini, em forma de chat, para que o usuário possa tirar dúvidas simples</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Plataforma para atendimento ao cliente e abertura de chamados</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -484,40 +496,7 @@
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -618,21 +597,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
       </left>
       <right style="thin">
@@ -654,19 +618,6 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,11 +838,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -899,61 +889,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -962,7 +910,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -973,7 +921,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -986,109 +934,118 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1110,6 +1067,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1126,6 +1103,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1141,6 +1138,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1156,6 +1173,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1171,6 +1208,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1186,6 +1243,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1201,6 +1278,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1488,16 +1585,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>126</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1620,16 +1717,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>126</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2516,7 +2613,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>1464189</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>304799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2546,8 +2643,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{056BFD53-8C90-4332-8B68-2F11BAE36F39}" name="Tabela1" displayName="Tabela1" ref="A2:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A2:G16" xr:uid="{056BFD53-8C90-4332-8B68-2F11BAE36F39}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{056BFD53-8C90-4332-8B68-2F11BAE36F39}" name="Tabela1" displayName="Tabela1" ref="A2:G18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A2:G18" xr:uid="{056BFD53-8C90-4332-8B68-2F11BAE36F39}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CA0F1531-D717-4C7A-8BD5-D5815D3A0D21}" name="Requisito" dataDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{B1CECBFD-E981-4981-8821-A53F4556E781}" name="Descrição" dataDxfId="5" dataCellStyle="Normal"/>
@@ -2878,10 +2975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C7FCD8-0F1D-4250-8221-026B8E3397EA}">
-  <dimension ref="A1:AA46"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2897,577 +2994,607 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="44.25" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="I1" s="63" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="I1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="65"/>
-      <c r="P1" s="47" t="s">
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="54"/>
+      <c r="P1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="30" t="s">
+      <c r="Q1" s="37"/>
+      <c r="R1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="45" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="61" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="P2" s="45" t="s">
+      <c r="N2" s="51"/>
+      <c r="P2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="105" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="28">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="29">
         <v>8</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="37" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="45" t="s">
+      <c r="P3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="29" t="s">
+      <c r="Q3" s="35"/>
+      <c r="R3" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="105" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="28">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="29">
         <v>8</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="32">
-        <f>SUMIFS(F3:F16, G3:G16, "Sprint 1")</f>
+      <c r="J4" s="27">
+        <f>SUMIFS(F3:F18, G3:G18, "Sprint 1")</f>
         <v>16</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="11">
         <v>16</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="8">
         <f>J7-K4</f>
-        <v>110</v>
-      </c>
-      <c r="M4" s="18">
+        <v>131</v>
+      </c>
+      <c r="M4" s="4">
         <v>16</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="9">
         <f>J7-M4</f>
-        <v>110</v>
-      </c>
-      <c r="P4" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="29" t="s">
+      <c r="Q4" s="35"/>
+      <c r="R4" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="105" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="28">
         <v>1</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="29">
         <v>5</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="34">
-        <f>SUMIFS(F3:F16, G3:G16, "Sprint 2")</f>
+      <c r="J5" s="26">
+        <f>SUMIFS(F3:F18, G3:G18, "Sprint 2")</f>
         <v>81</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="12">
         <v>74</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="8">
         <f>L4-K5</f>
+        <v>57</v>
+      </c>
+      <c r="M5" s="4">
+        <v>68</v>
+      </c>
+      <c r="N5" s="9">
+        <f>N4-M5</f>
+        <v>63</v>
+      </c>
+      <c r="P5" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="18">
+      <c r="Q5" s="35"/>
+      <c r="R5" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="105" customHeight="1">
+      <c r="A6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="29">
+        <v>13</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="25">
+        <f>SUMIFS(F3:F18, G3:G18, "Sprint 3")</f>
+        <v>50</v>
+      </c>
+      <c r="K6" s="13">
+        <v>36</v>
+      </c>
+      <c r="L6" s="7">
+        <f>L5-K6</f>
+        <v>21</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <f>N5-M6</f>
+        <v>63</v>
+      </c>
+      <c r="P6" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="117" customHeight="1">
+      <c r="A7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="28">
+        <v>1</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="29">
+        <v>13</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="38">
+        <f>SUM(J4:J6)</f>
+        <v>147</v>
+      </c>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
+      <c r="P7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="105" customHeight="1">
+      <c r="A8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="28">
+        <v>2</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="29">
+        <v>13</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="41">
+        <f>QUOTIENT(J7,3)</f>
+        <v>49</v>
+      </c>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="42"/>
+      <c r="P8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="105" customHeight="1">
+      <c r="A9" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="28">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="29">
+        <v>13</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+    </row>
+    <row r="10" spans="1:27" ht="105" customHeight="1">
+      <c r="A10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="28">
+        <v>1</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="29">
+        <v>21</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="105" customHeight="1">
+      <c r="A11" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="28">
+        <v>1</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="29">
+        <v>5</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="105" customHeight="1">
+      <c r="A12" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="28">
+        <v>2</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="29">
+        <v>3</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="105" customHeight="1">
+      <c r="A13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="28">
+        <v>3</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="29">
+        <v>8</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="105" customHeight="1">
+      <c r="A14" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="23">
-        <f>N4-M5</f>
-        <v>42</v>
-      </c>
-      <c r="P5" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="105" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="C14" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="28">
+        <v>2</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="29">
+        <v>8</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="105" customHeight="1">
+      <c r="A15" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="28">
+        <v>2</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="29">
+        <v>3</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="105" customHeight="1">
+      <c r="A16" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D16" s="28">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="29">
+        <v>8</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="105" customHeight="1">
+      <c r="A17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="28">
+        <v>3</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="29">
+        <v>5</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="105" customHeight="1">
+      <c r="A18" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="32">
+        <v>1</v>
+      </c>
+      <c r="E18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F18" s="33">
         <v>13</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="35" t="s">
+      <c r="G18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="36">
-        <f>SUMIFS(F3:F16, G3:G16, "Sprint 3")</f>
-        <v>29</v>
-      </c>
-      <c r="K6" s="27">
-        <v>36</v>
-      </c>
-      <c r="L6" s="21">
-        <f>L5-K6</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="19">
-        <v>0</v>
-      </c>
-      <c r="N6" s="24">
-        <f>N5-M6</f>
-        <v>42</v>
-      </c>
-      <c r="P6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="117" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="44">
-        <v>13</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="49">
-        <f>SUM(J4:J6)</f>
-        <v>126</v>
-      </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
-      <c r="P7" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="105" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="12">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="43">
-        <v>13</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="52">
-        <f>QUOTIENT(J7,3)</f>
-        <v>42</v>
-      </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="53"/>
-      <c r="P8" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="105" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="15">
-        <v>1</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="43">
-        <v>13</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-    </row>
-    <row r="10" spans="1:27" ht="105" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="44">
-        <v>21</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="105" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="44">
-        <v>5</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="105" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="16">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="43">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="105" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="43">
-        <v>8</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="105" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="16">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="43">
-        <v>8</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="105" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="10">
-        <v>2</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="42">
-        <v>3</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="105" customHeight="1">
-      <c r="A16" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="10">
-        <v>3</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="42">
-        <v>5</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="105" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="105" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="105" customHeight="1">
+    </row>
+    <row r="19" spans="1:7" ht="105" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -3475,7 +3602,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="105" customHeight="1">
+    <row r="20" spans="1:7" ht="105" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -3483,7 +3610,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="105" customHeight="1">
+    <row r="21" spans="1:7" ht="105" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3491,7 +3618,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="105" customHeight="1">
+    <row r="22" spans="1:7" ht="105" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3499,7 +3626,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="105" customHeight="1">
+    <row r="23" spans="1:7" ht="105" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3507,7 +3634,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="105" customHeight="1">
+    <row r="24" spans="1:7" ht="105" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3515,7 +3642,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="105" customHeight="1">
+    <row r="25" spans="1:7" ht="105" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3523,7 +3650,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="105" customHeight="1">
+    <row r="26" spans="1:7" ht="105" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3531,7 +3658,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="105" customHeight="1">
+    <row r="27" spans="1:7" ht="105" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3539,7 +3666,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="105" customHeight="1">
+    <row r="28" spans="1:7" ht="105" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3547,7 +3674,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="105" customHeight="1">
+    <row r="29" spans="1:7" ht="105" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3555,7 +3682,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="105" customHeight="1">
+    <row r="30" spans="1:7" ht="105" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3563,7 +3690,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7" ht="105" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3571,7 +3698,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3690,6 +3817,14 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -3711,7 +3846,7 @@
     <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16" xr:uid="{37480E56-EA93-432A-ABE3-38233953F318}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G18" xr:uid="{37480E56-EA93-432A-ABE3-38233953F318}">
       <formula1>$I$4:$I$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -3724,6 +3859,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
@@ -3731,7 +3875,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080A269BF505ACD4B84A4678488096051" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f655fa647c6606e084716ad29b00db24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32844186-265b-4793-912a-671da4ac73b2" xmlns:ns4="97232348-304c-4ff8-affc-b0d6bfd913f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="43fd82a98f63819bf2f7aba644d7bb9a" ns3:_="" ns4:_="">
     <xsd:import namespace="32844186-265b-4793-912a-671da4ac73b2"/>
@@ -3952,23 +4096,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F4195D8-5F0A-4AC8-B1B5-4DE783C90FD6}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89855FBC-43DA-45D7-BC2C-012429D7A188}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3723D44E-12E8-4DD0-A6E2-C8E98872AB14}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F4195D8-5F0A-4AC8-B1B5-4DE783C90FD6}"/>
 </file>
</xml_diff>